<commit_message>
Arreglo error y ejercicio a terminado
</commit_message>
<xml_diff>
--- a/Practica5/Ejercicio23.xlsx
+++ b/Practica5/Ejercicio23.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Massimo\Desktop\UNLP\2do año\segundo\ISO\Practica5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A560781B-9361-4C91-A91F-82D2D503D4EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F11E6357-5C32-408B-8895-5FEE4FD36FA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{2E33B7E5-167B-4C5B-BE4E-2B9B43FF97C9}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="44">
   <si>
     <t>A1</t>
   </si>
@@ -142,6 +142,30 @@
   </si>
   <si>
     <t>X</t>
+  </si>
+  <si>
+    <t>Sec chance</t>
+  </si>
+  <si>
+    <t>A1*</t>
+  </si>
+  <si>
+    <t>B2*</t>
+  </si>
+  <si>
+    <t>B4*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A1 </t>
+  </si>
+  <si>
+    <t>C4*</t>
+  </si>
+  <si>
+    <t>C1*</t>
+  </si>
+  <si>
+    <t>A4*</t>
   </si>
 </sst>
 </file>
@@ -206,13 +230,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -527,17 +553,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B83217B0-F6B2-47D4-BD68-4DFA3E7ABC49}">
-  <dimension ref="A1:AH13"/>
+  <dimension ref="A1:AH27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AC13" sqref="AC13"/>
+      <selection activeCell="AA10" sqref="AA10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8" customWidth="1"/>
-    <col min="2" max="27" width="3.28515625" customWidth="1"/>
-    <col min="28" max="34" width="3.5703125" customWidth="1"/>
+    <col min="2" max="34" width="4.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.25">
@@ -632,10 +657,10 @@
         <v>30</v>
       </c>
       <c r="AE1" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="AF1" s="4" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="AG1" s="4" t="s">
         <v>33</v>
@@ -1116,13 +1141,13 @@
         <v>28</v>
       </c>
       <c r="AE6" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="AF6" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AG6" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
+      </c>
+      <c r="AG6" s="1">
+        <v>9</v>
       </c>
       <c r="AH6" s="1"/>
     </row>
@@ -1295,10 +1320,10 @@
         <v>0</v>
       </c>
       <c r="AF8" s="1" t="s">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="AG8" s="1" t="s">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="AH8" s="1"/>
     </row>
@@ -1384,9 +1409,7 @@
       <c r="AE9" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AF9" s="1" t="s">
-        <v>35</v>
-      </c>
+      <c r="AF9" s="1"/>
       <c r="AG9" s="1"/>
       <c r="AH9" s="1"/>
     </row>
@@ -1595,6 +1618,1060 @@
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
     </row>
+    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="K15" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="L15" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="M15" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="N15" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="O15" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="P15" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q15" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="R15" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="S15" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="T15" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="U15" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="V15" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="W15" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="X15" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y15" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="Z15" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA15" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB15" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="AC15" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="AD15" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="AE15" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="AF15" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="AG15" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="AH15" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="J16" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="K16" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="L16" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="M16" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="N16" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="O16" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="P16" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q16" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="R16" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="S16" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="T16" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="U16" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="V16" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="W16" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="X16" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y16" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="Z16" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA16" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="AB16" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="AC16" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="AD16" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="AE16" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="AF16" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="AG16" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="AH16" s="1"/>
+    </row>
+    <row r="17" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="J17" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K17" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="L17" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="M17" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="N17" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="O17" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="P17" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q17" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="R17" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="S17" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="T17" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="U17" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="V17" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="W17" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="X17" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y17" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z17" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA17" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB17" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC17" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD17" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="AE17" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF17" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="AG17" s="6"/>
+      <c r="AH17" s="1"/>
+    </row>
+    <row r="18" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="I18" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="J18" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="K18" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L18" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="M18" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="N18" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="O18" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="P18" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q18" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="R18" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="S18" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="T18" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="U18" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="V18" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="W18" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="X18" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y18" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z18" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="AA18" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB18" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC18" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD18" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE18" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF18" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="AG18" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH18" s="1"/>
+    </row>
+    <row r="19" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="J19" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="K19" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="L19" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="M19" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="N19" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="O19" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="P19" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q19" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="R19" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="S19" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="T19" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="U19" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="V19" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="W19" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="X19" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y19" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z19" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA19" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB19" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="AC19" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="AD19" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="AE19" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="AF19" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG19" s="6"/>
+      <c r="AH19" s="1"/>
+    </row>
+    <row r="20" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I20" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="J20" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="K20" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="L20" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="M20" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="N20" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="O20" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="P20" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q20" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="R20" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="S20" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="T20" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="U20" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="V20" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="W20" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="X20" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y20" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z20" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA20" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB20" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="AC20" s="6"/>
+      <c r="AD20" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="AE20" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF20" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="AG20" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="AH20" s="1"/>
+    </row>
+    <row r="21" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I21" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J21" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="K21" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="L21" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="M21" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="N21" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="O21" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="P21" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q21" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="R21" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="S21" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="T21" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="U21" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="V21" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="W21" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="X21" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y21" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z21" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="AA21" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB21" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="AC21" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="AD21" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="AE21" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="AF21" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="AG21" s="6"/>
+      <c r="AH21" s="1"/>
+    </row>
+    <row r="22" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J22" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="K22" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L22" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="M22" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="N22" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="O22" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="P22" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q22" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="R22" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="S22" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="T22" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="U22" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="V22" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="W22" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="X22" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y22" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z22" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA22" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB22" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC22" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD22" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE22" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="AF22" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="AG22" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH22" s="1"/>
+    </row>
+    <row r="23" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H23" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="I23" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="M23" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="N23" s="6"/>
+      <c r="O23" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="P23" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q23" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="R23" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="S23" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="T23" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="U23" s="6"/>
+      <c r="V23" s="6"/>
+      <c r="W23" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="X23" s="6"/>
+      <c r="Y23" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z23" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA23" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="AB23" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC23" s="6"/>
+      <c r="AD23" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="AE23" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF23" s="6"/>
+      <c r="AG23" s="6"/>
+      <c r="AH23" s="1"/>
+    </row>
+    <row r="24" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J24" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="K24" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="L24" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="M24" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="N24" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="O24" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="P24" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q24" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="R24" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="S24" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="T24" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="U24" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="V24" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="W24" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="X24" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y24" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z24" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA24" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB24" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="AC24" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="AD24" s="6"/>
+      <c r="AE24" s="6"/>
+      <c r="AF24" s="6"/>
+      <c r="AG24" s="6"/>
+      <c r="AH24" s="1"/>
+    </row>
+    <row r="25" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B25" s="3">
+        <v>1</v>
+      </c>
+      <c r="C25" s="3">
+        <v>3</v>
+      </c>
+      <c r="D25" s="3">
+        <v>1</v>
+      </c>
+      <c r="E25" s="3">
+        <v>2</v>
+      </c>
+      <c r="F25" s="3">
+        <v>4</v>
+      </c>
+      <c r="G25" s="3">
+        <v>1</v>
+      </c>
+      <c r="H25" s="3">
+        <v>5</v>
+      </c>
+      <c r="I25" s="3">
+        <v>1</v>
+      </c>
+      <c r="J25" s="3">
+        <v>4</v>
+      </c>
+      <c r="K25" s="6">
+        <v>7</v>
+      </c>
+      <c r="L25" s="6">
+        <v>9</v>
+      </c>
+      <c r="M25" s="6">
+        <v>4</v>
+      </c>
+      <c r="V25" s="7"/>
+      <c r="AF25" s="7"/>
+    </row>
+    <row r="26" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B26" s="3">
+        <v>2</v>
+      </c>
+      <c r="C26" s="3">
+        <v>4</v>
+      </c>
+      <c r="D26" s="3">
+        <v>6</v>
+      </c>
+      <c r="E26" s="3">
+        <v>2</v>
+      </c>
+      <c r="F26" s="3">
+        <v>4</v>
+      </c>
+      <c r="G26" s="3">
+        <v>1</v>
+      </c>
+      <c r="H26" s="3">
+        <v>8</v>
+      </c>
+      <c r="I26" s="3">
+        <v>3</v>
+      </c>
+      <c r="J26" s="3">
+        <v>1</v>
+      </c>
+      <c r="K26" s="3">
+        <v>8</v>
+      </c>
+      <c r="L26" s="6"/>
+      <c r="M26" s="6"/>
+      <c r="V26" s="7"/>
+      <c r="AF26" s="7"/>
+    </row>
+    <row r="27" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B27" s="3">
+        <v>1</v>
+      </c>
+      <c r="C27" s="3">
+        <v>2</v>
+      </c>
+      <c r="D27" s="3">
+        <v>4</v>
+      </c>
+      <c r="E27" s="3">
+        <v>8</v>
+      </c>
+      <c r="F27" s="3">
+        <v>6</v>
+      </c>
+      <c r="G27" s="3">
+        <v>1</v>
+      </c>
+      <c r="H27" s="3">
+        <v>4</v>
+      </c>
+      <c r="I27" s="3">
+        <v>1</v>
+      </c>
+      <c r="J27" s="6"/>
+      <c r="K27" s="6"/>
+      <c r="L27" s="6"/>
+      <c r="M27" s="6"/>
+      <c r="V27" s="7"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>